<commit_message>
Add filter for non-positive numerator values
</commit_message>
<xml_diff>
--- a/Projects/NESTLEUS/Data/Nestle Waters Test Sessions.xlsx
+++ b/Projects/NESTLEUS/Data/Nestle Waters Test Sessions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="60">
   <si>
     <t xml:space="preserve">Session_uid</t>
   </si>
@@ -28,163 +28,178 @@
     <t xml:space="preserve">Status</t>
   </si>
   <si>
+    <t xml:space="preserve">00f85f4b-530b-4350-86ce-c0268abce9b8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03c096f9-21a1-4468-b6a5-49421a576c92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04aaf0a9-fe95-4317-8743-172ea1b51588</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07db7d13-0dd9-48fe-9637-692da4599bc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08cbe1f4-0924-494c-85e5-ebc6849694cf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0925166a-0a4f-4c13-84a5-a93f425d3ea9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0d71ea3c-6430-488e-88e1-dd83ef64d2c9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0eb0ce82-fa60-4450-aeb9-a3adc65ffab8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0f3fb7d2-1390-4d51-8b4e-6aca65025b63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">143e4f5a-0f2c-41e3-8b15-2abedf32a148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19d19213-fdd0-4bab-8fce-a27b201588d9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1db75134-b5e8-428b-b1a8-8cb29b10c2f5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1f9d5638-d8f4-4f74-a588-7999459af4bf</t>
+  </si>
+  <si>
     <t xml:space="preserve">2455f53c-4b25-4059-ae00-aa7ca2c7edf8</t>
   </si>
   <si>
-    <t xml:space="preserve">Completed</t>
+    <t xml:space="preserve">24e7b2b2-3436-4abf-9f3d-f67a3a29896c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2c1694f8-beb1-4f1d-8d5a-016a616564d2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32fe90c2-5ba4-44c9-aec7-aef21fa77a9b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3c760307-76b6-4434-8590-dbfcf75d7d1e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3d72d6a4-1066-4723-8e00-53d4143f3dda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43f1adaf-ab88-45c6-a569-c7904a0a475b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45e3f6f8-7ad3-4e49-87ee-bc05a139227c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">494442ed-b519-45b2-8bfe-5313ea0fef13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4d50c64e-0219-418a-a9c9-23e06f28b90f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4d5e7efc-8d46-4eff-9254-81d3d7562537</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5aeecd74-61e6-413a-9fe1-db6160d38219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5d6c2b97-4f7b-470e-a7de-1334bcc3f08f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6925a0d9-70c9-4b31-b485-230db54b46ed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6a02f170-859d-4685-a1e9-d717c47cd530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6b893fd0-84d6-4902-85df-166ed80faa0e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6fc47e9f-4481-4211-8730-fa964e9d035b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">721db695-1de6-4d12-b4b6-bd8953a69750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">763cec6c-7acd-4143-9eb4-1ff720e467fb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7d444837-b207-449e-9208-801886ba064c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7dcb8c8b-3a1e-452a-a5d7-d1e4fecb1bd2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">804c311a-a9db-4af8-9197-99085592c74b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85ad84df-e4e6-458b-880d-b8247bceaf11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86a343bc-1bd2-411a-9f3e-2550cd75a66c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89094ff2-79b7-40d2-8edd-3ff72ce84b72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91ae83e9-ecbc-44d5-a93d-2c601013b0df</t>
+  </si>
+  <si>
+    <t xml:space="preserve">982a1300-575e-42ef-93a2-9ff25e2e9c30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a3bd12fa-1088-496e-8688-fa221df637be</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bc8ad00d-8025-4eb3-a9e8-56f8aad34420</t>
+  </si>
+  <si>
+    <t xml:space="preserve">befc4f71-e816-4546-8b5d-47ae4b61dcd9</t>
   </si>
   <si>
     <t xml:space="preserve">bf8e28a4-2680-48a0-a978-a03715f81181</t>
   </si>
   <si>
-    <t xml:space="preserve">1db75134-b5e8-428b-b1a8-8cb29b10c2f5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">721db695-1de6-4d12-b4b6-bd8953a69750</t>
-  </si>
-  <si>
-    <t xml:space="preserve">763cec6c-7acd-4143-9eb4-1ff720e467fb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">85ad84df-e4e6-458b-880d-b8247bceaf11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6b893fd0-84d6-4902-85df-166ed80faa0e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32fe90c2-5ba4-44c9-aec7-aef21fa77a9b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">804c311a-a9db-4af8-9197-99085592c74b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a3bd12fa-1088-496e-8688-fa221df637be</t>
-  </si>
-  <si>
-    <t xml:space="preserve">89094ff2-79b7-40d2-8edd-3ff72ce84b72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">befc4f71-e816-4546-8b5d-47ae4b61dcd9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43f1adaf-ab88-45c6-a569-c7904a0a475b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45e3f6f8-7ad3-4e49-87ee-bc05a139227c</t>
+    <t xml:space="preserve">c18e11bd-d3e8-43fc-999c-4d61c5701a13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d0b2f08d-f44e-4d99-8228-ecb95dd1e620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deac0ba2-de4a-497f-a9dd-94c050c4ca6d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e0759078-f182-4c8d-8150-fc9b505db1e5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e2291f44-5566-419e-bc80-040eb192a540</t>
   </si>
   <si>
     <t xml:space="preserve">e89d0ee5-168e-4a68-81f3-523ddb6c93c4</t>
   </si>
   <si>
-    <t xml:space="preserve">6925a0d9-70c9-4b31-b485-230db54b46ed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86a343bc-1bd2-411a-9f3e-2550cd75a66c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24e7b2b2-3436-4abf-9f3d-f67a3a29896c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00f85f4b-530b-4350-86ce-c0268abce9b8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3c760307-76b6-4434-8590-dbfcf75d7d1e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4d5e7efc-8d46-4eff-9254-81d3d7562537</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bc8ad00d-8025-4eb3-a9e8-56f8aad34420</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deac0ba2-de4a-497f-a9dd-94c050c4ca6d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7dcb8c8b-3a1e-452a-a5d7-d1e4fecb1bd2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6fc47e9f-4481-4211-8730-fa964e9d035b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e2291f44-5566-419e-bc80-040eb192a540</t>
-  </si>
-  <si>
     <t xml:space="preserve">f14324ed-2080-4bbb-9321-04a5e7502634</t>
   </si>
   <si>
+    <t xml:space="preserve">fac7d625-3d44-4f9b-b52d-1b089f66e12b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fbc8e854-f462-4f15-96a5-01e54fdf1465</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fc57c4b9-a01f-4198-8669-8016928d068f</t>
+  </si>
+  <si>
     <t xml:space="preserve">fcba7974-cce5-4dc9-970a-15b08a564859</t>
   </si>
   <si>
-    <t xml:space="preserve">2c1694f8-beb1-4f1d-8d5a-016a616564d2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d0b2f08d-f44e-4d99-8228-ecb95dd1e620</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0eb0ce82-fa60-4450-aeb9-a3adc65ffab8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7d444837-b207-449e-9208-801886ba064c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4d50c64e-0219-418a-a9c9-23e06f28b90f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">982a1300-575e-42ef-93a2-9ff25e2e9c30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e0759078-f182-4c8d-8150-fc9b505db1e5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5aeecd74-61e6-413a-9fe1-db6160d38219</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1f9d5638-d8f4-4f74-a588-7999459af4bf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6a02f170-859d-4685-a1e9-d717c47cd530</t>
-  </si>
-  <si>
-    <t xml:space="preserve">143e4f5a-0f2c-41e3-8b15-2abedf32a148</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5d6c2b97-4f7b-470e-a7de-1334bcc3f08f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c18e11bd-d3e8-43fc-999c-4d61c5701a13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fac7d625-3d44-4f9b-b52d-1b089f66e12b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">494442ed-b519-45b2-8bfe-5313ea0fef13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0f3fb7d2-1390-4d51-8b4e-6aca65025b63</t>
+    <t xml:space="preserve">ff474ba2-fb55-422a-adb1-44ae3410bbf3</t>
   </si>
   <si>
     <t xml:space="preserve">ffabc90f-2ee3-47ca-9ece-7f03be04bfbd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19d19213-fdd0-4bab-8fce-a27b201588d9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fbc8e854-f462-4f15-96a5-01e54fdf1465</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3d72d6a4-1066-4723-8e00-53d4143f3dda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0d71ea3c-6430-488e-88e1-dd83ef64d2c9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">91ae83e9-ecbc-44d5-a93d-2c601013b0df</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fc57c4b9-a01f-4198-8669-8016928d068f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ff474ba2-fb55-422a-adb1-44ae3410bbf3</t>
   </si>
 </sst>
 </file>
@@ -294,15 +309,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.7773279352227"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
@@ -315,7 +330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -323,47 +338,47 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -371,7 +386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -379,7 +394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -387,7 +402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -395,7 +410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -403,7 +418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -411,7 +426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -419,7 +434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -427,7 +442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -435,7 +450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
@@ -443,7 +458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -451,7 +466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -459,7 +474,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -467,7 +482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -475,7 +490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -483,7 +498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
@@ -491,7 +506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -499,7 +514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -507,7 +522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
@@ -515,7 +530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>28</v>
       </c>
@@ -523,7 +538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>29</v>
       </c>
@@ -531,7 +546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -539,7 +554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>31</v>
       </c>
@@ -547,7 +562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>32</v>
       </c>
@@ -555,7 +570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>33</v>
       </c>
@@ -563,7 +578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>34</v>
       </c>
@@ -571,7 +586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>35</v>
       </c>
@@ -579,7 +594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>36</v>
       </c>
@@ -587,7 +602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
         <v>37</v>
       </c>
@@ -595,7 +610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
         <v>38</v>
       </c>
@@ -603,7 +618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>39</v>
       </c>
@@ -611,7 +626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>40</v>
       </c>
@@ -619,7 +634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>41</v>
       </c>
@@ -627,7 +642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>42</v>
       </c>
@@ -635,7 +650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
@@ -643,7 +658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
@@ -651,7 +666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
         <v>45</v>
       </c>
@@ -659,7 +674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
@@ -667,7 +682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
         <v>47</v>
       </c>
@@ -675,7 +690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
         <v>48</v>
       </c>
@@ -683,7 +698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
         <v>49</v>
       </c>
@@ -691,7 +706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
         <v>50</v>
       </c>
@@ -699,7 +714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
@@ -715,8 +730,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -724,13 +739,54 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Add check for water aisles and water displays
</commit_message>
<xml_diff>
--- a/Projects/NESTLEUS/Data/Nestle Waters Test Sessions.xlsx
+++ b/Projects/NESTLEUS/Data/Nestle Waters Test Sessions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
   <si>
     <t xml:space="preserve">Session_uid</t>
   </si>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">143e4f5a-0f2c-41e3-8b15-2abedf32a148</t>
   </si>
   <si>
+    <t xml:space="preserve">177c0014-46e6-41cc-a35d-2e2c462a2537</t>
+  </si>
+  <si>
     <t xml:space="preserve">19d19213-fdd0-4bab-8fce-a27b201588d9</t>
   </si>
   <si>
@@ -82,6 +85,9 @@
     <t xml:space="preserve">32fe90c2-5ba4-44c9-aec7-aef21fa77a9b</t>
   </si>
   <si>
+    <t xml:space="preserve">359b4a0d-fb45-460c-9736-7737ccf6c45a</t>
+  </si>
+  <si>
     <t xml:space="preserve">3c760307-76b6-4434-8590-dbfcf75d7d1e</t>
   </si>
   <si>
@@ -103,6 +109,9 @@
     <t xml:space="preserve">4d5e7efc-8d46-4eff-9254-81d3d7562537</t>
   </si>
   <si>
+    <t xml:space="preserve">50730f02-8ac1-4918-bc48-acf6fc02dfb6</t>
+  </si>
+  <si>
     <t xml:space="preserve">5aeecd74-61e6-413a-9fe1-db6160d38219</t>
   </si>
   <si>
@@ -115,6 +124,9 @@
     <t xml:space="preserve">6a02f170-859d-4685-a1e9-d717c47cd530</t>
   </si>
   <si>
+    <t xml:space="preserve">6a54ba4b-c2da-4939-bb70-79101f4016e1</t>
+  </si>
+  <si>
     <t xml:space="preserve">6b893fd0-84d6-4902-85df-166ed80faa0e</t>
   </si>
   <si>
@@ -167,6 +179,9 @@
   </si>
   <si>
     <t xml:space="preserve">d0b2f08d-f44e-4d99-8228-ecb95dd1e620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d318462b-324d-4426-abcf-21d191c6170d</t>
   </si>
   <si>
     <t xml:space="preserve">deac0ba2-de4a-497f-a9dd-94c050c4ca6d</t>
@@ -275,7 +290,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -290,6 +305,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -312,12 +331,12 @@
   <dimension ref="A1:B65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0971659919028"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
@@ -411,7 +430,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="0" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -475,7 +494,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -539,7 +558,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="0" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -579,7 +598,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -731,7 +750,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="0" t="s">
         <v>53</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -754,8 +773,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3" t="s">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -771,7 +790,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -786,6 +805,48 @@
         <v>3</v>
       </c>
     </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>